<commit_message>
Up to date for July 2017
</commit_message>
<xml_diff>
--- a/Evolution Sim Spreadsheet.xlsx
+++ b/Evolution Sim Spreadsheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>nstar</t>
   </si>
@@ -59,9 +59,6 @@
     <t>k</t>
   </si>
   <si>
-    <t>Done?</t>
-  </si>
-  <si>
     <t>Replicate</t>
   </si>
   <si>
@@ -84,6 +81,39 @@
   </si>
   <si>
     <t>Env Change</t>
+  </si>
+  <si>
+    <t>Where?</t>
+  </si>
+  <si>
+    <t>Status?</t>
+  </si>
+  <si>
+    <t>CLV</t>
+  </si>
+  <si>
+    <t>Matt</t>
+  </si>
+  <si>
+    <t>Lab</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Running (active)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Started (not currently running) </t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>zneut_init</t>
   </si>
 </sst>
 </file>
@@ -99,7 +129,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,6 +151,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -146,12 +182,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -440,21 +478,23 @@
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="7.6640625" customWidth="1"/>
-    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -470,48 +510,50 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J1" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>20</v>
       </c>
@@ -527,11 +569,23 @@
       <c r="E2">
         <v>50</v>
       </c>
+      <c r="F2">
+        <v>-1</v>
+      </c>
+      <c r="G2">
+        <v>0.25</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
       <c r="J2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -540,29 +594,26 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>5000</v>
       </c>
       <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>400</v>
-      </c>
-      <c r="R2">
-        <v>5000</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U2" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="2"/>
+      <c r="S2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20</v>
       </c>
@@ -578,11 +629,23 @@
       <c r="E3">
         <v>50</v>
       </c>
+      <c r="F3">
+        <v>-1</v>
+      </c>
+      <c r="G3">
+        <v>0.25</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
       <c r="J3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -591,29 +654,27 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>5000</v>
       </c>
       <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>400</v>
-      </c>
-      <c r="R3">
-        <v>5000</v>
-      </c>
-      <c r="S3">
         <v>2</v>
       </c>
-      <c r="T3" t="s">
-        <v>17</v>
-      </c>
-      <c r="U3" s="2"/>
+      <c r="Q3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="2"/>
+      <c r="S3" t="s">
+        <v>21</v>
+      </c>
+      <c r="V3" s="2"/>
+      <c r="W3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20</v>
       </c>
@@ -629,11 +690,23 @@
       <c r="E4">
         <v>50</v>
       </c>
+      <c r="F4">
+        <v>-1</v>
+      </c>
+      <c r="G4">
+        <v>0.25</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
       <c r="J4">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -642,29 +715,27 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>5000</v>
       </c>
       <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>400</v>
-      </c>
-      <c r="R4">
-        <v>5000</v>
-      </c>
-      <c r="S4">
         <v>3</v>
       </c>
-      <c r="T4" t="s">
-        <v>17</v>
-      </c>
-      <c r="U4" s="2"/>
+      <c r="Q4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="2"/>
+      <c r="S4" t="s">
+        <v>21</v>
+      </c>
+      <c r="V4" s="3"/>
+      <c r="W4" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20</v>
       </c>
@@ -680,30 +751,52 @@
       <c r="E5">
         <v>50</v>
       </c>
+      <c r="F5">
+        <v>-1.007749</v>
+      </c>
+      <c r="G5">
+        <v>0.25140699999999999</v>
+      </c>
+      <c r="H5">
+        <v>1.0028919999999999</v>
+      </c>
+      <c r="I5">
+        <v>1.5401659999999999E-3</v>
+      </c>
+      <c r="J5">
+        <v>3.428726E-2</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
       <c r="N5">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>15000</v>
       </c>
       <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>400</v>
-      </c>
-      <c r="R5">
-        <v>20000</v>
-      </c>
-      <c r="S5">
-        <v>1</v>
-      </c>
-      <c r="T5" t="s">
-        <v>18</v>
-      </c>
-      <c r="U5" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>17</v>
+      </c>
+      <c r="R5" s="2"/>
+      <c r="S5" t="s">
+        <v>21</v>
+      </c>
+      <c r="V5" s="6"/>
+      <c r="W5" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20</v>
       </c>
@@ -719,30 +812,52 @@
       <c r="E6">
         <v>50</v>
       </c>
+      <c r="F6">
+        <v>-1.007749</v>
+      </c>
+      <c r="G6">
+        <v>0.25140699999999999</v>
+      </c>
+      <c r="H6">
+        <v>1.0028919999999999</v>
+      </c>
+      <c r="I6">
+        <v>1.5401659999999999E-3</v>
+      </c>
+      <c r="J6">
+        <v>3.428726E-2</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1E-4</v>
+      </c>
       <c r="N6">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>15000</v>
       </c>
       <c r="P6">
-        <v>1E-4</v>
-      </c>
-      <c r="Q6">
-        <v>400</v>
-      </c>
-      <c r="R6">
-        <v>20000</v>
-      </c>
-      <c r="S6">
-        <v>1</v>
-      </c>
-      <c r="T6" t="s">
-        <v>19</v>
-      </c>
-      <c r="U6" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>18</v>
+      </c>
+      <c r="R6" s="3"/>
+      <c r="S6" t="s">
+        <v>21</v>
+      </c>
+      <c r="V6" s="4"/>
+      <c r="W6" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>20</v>
       </c>
@@ -758,30 +873,48 @@
       <c r="E7">
         <v>50</v>
       </c>
+      <c r="F7">
+        <v>-0.99540740000000005</v>
+      </c>
+      <c r="G7">
+        <v>0.2523705</v>
+      </c>
+      <c r="H7">
+        <v>1.001571</v>
+      </c>
+      <c r="I7">
+        <v>-6.1947860000000001E-4</v>
+      </c>
+      <c r="J7">
+        <v>-0.26853399999999999</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
       <c r="N7">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="O7">
-        <v>1</v>
+        <v>15000</v>
       </c>
       <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>400</v>
-      </c>
-      <c r="R7">
-        <v>20000</v>
-      </c>
-      <c r="S7">
         <v>2</v>
       </c>
-      <c r="T7" t="s">
-        <v>18</v>
-      </c>
-      <c r="U7" s="4"/>
+      <c r="Q7" t="s">
+        <v>17</v>
+      </c>
+      <c r="R7" s="2"/>
+      <c r="S7" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>20</v>
       </c>
@@ -797,30 +930,45 @@
       <c r="E8">
         <v>50</v>
       </c>
+      <c r="F8">
+        <v>-0.99540740000000005</v>
+      </c>
+      <c r="G8">
+        <v>0.2523705</v>
+      </c>
+      <c r="H8">
+        <v>1.001571</v>
+      </c>
+      <c r="I8">
+        <v>-6.1947860000000001E-4</v>
+      </c>
+      <c r="J8">
+        <v>-0.26853399999999999</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1E-4</v>
+      </c>
       <c r="N8">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="O8">
-        <v>1</v>
+        <v>15000</v>
       </c>
       <c r="P8">
-        <v>1E-4</v>
-      </c>
-      <c r="Q8">
-        <v>400</v>
-      </c>
-      <c r="R8">
-        <v>20000</v>
-      </c>
-      <c r="S8">
         <v>2</v>
       </c>
-      <c r="T8" t="s">
-        <v>19</v>
-      </c>
-      <c r="U8" s="4"/>
+      <c r="Q8" t="s">
+        <v>18</v>
+      </c>
+      <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20</v>
       </c>
@@ -836,30 +984,48 @@
       <c r="E9">
         <v>50</v>
       </c>
+      <c r="F9">
+        <v>-1.003652</v>
+      </c>
+      <c r="G9">
+        <v>0.25534449999999997</v>
+      </c>
+      <c r="H9">
+        <v>1.002667</v>
+      </c>
+      <c r="I9">
+        <v>6.2326710000000004E-3</v>
+      </c>
+      <c r="J9">
+        <v>1.294203</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
       <c r="N9">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="O9">
-        <v>1</v>
+        <v>15000</v>
       </c>
       <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>400</v>
-      </c>
-      <c r="R9">
-        <v>20000</v>
-      </c>
-      <c r="S9">
         <v>3</v>
       </c>
-      <c r="T9" t="s">
-        <v>18</v>
-      </c>
-      <c r="U9" s="3"/>
+      <c r="Q9" t="s">
+        <v>17</v>
+      </c>
+      <c r="R9" s="3"/>
+      <c r="S9" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20</v>
       </c>
@@ -875,28 +1041,46 @@
       <c r="E10">
         <v>50</v>
       </c>
+      <c r="F10">
+        <v>-1.003652</v>
+      </c>
+      <c r="G10">
+        <v>0.25534449999999997</v>
+      </c>
+      <c r="H10">
+        <v>1.002667</v>
+      </c>
+      <c r="I10">
+        <v>6.2326710000000004E-3</v>
+      </c>
+      <c r="J10">
+        <v>1.294203</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1E-4</v>
+      </c>
       <c r="N10">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="O10">
-        <v>1</v>
+        <v>15000</v>
       </c>
       <c r="P10">
-        <v>1E-4</v>
-      </c>
-      <c r="Q10">
-        <v>400</v>
-      </c>
-      <c r="R10">
-        <v>20000</v>
-      </c>
-      <c r="S10">
         <v>3</v>
       </c>
-      <c r="T10" t="s">
-        <v>19</v>
-      </c>
-      <c r="U10" s="4"/>
+      <c r="Q10" t="s">
+        <v>18</v>
+      </c>
+      <c r="R10" s="3"/>
+      <c r="S10" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>